<commit_message>
some minor changes for the revision
</commit_message>
<xml_diff>
--- a/RCode/VerificationMatrix.xlsx
+++ b/RCode/VerificationMatrix.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\MatlabCode\projects\HMASandbox\HMA_Sandbox\Butterfly\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\R\ButterflyPublicationRepo\GRNP_2020\RCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154C145D-B186-4E95-833B-61E94EF147FD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE95B54-88F3-40B3-A476-F854E0E18B96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="86">
   <si>
     <t>File/Function</t>
   </si>
@@ -265,6 +265,24 @@
   </si>
   <si>
     <t>This file is copied from PreseqR and slightly modified. The performance gain vs accuracy loss is tested with TCR0004.</t>
+  </si>
+  <si>
+    <t>upSampleAndGetMeanExprPreSeqPreseq</t>
+  </si>
+  <si>
+    <t>Used in figure 5 - the results look reasonable, no further tests have been done. The code is close to identical to that of upSampleAndGetMeanExprPreSeqZTNB</t>
+  </si>
+  <si>
+    <t>BinomialDownsampling.R</t>
+  </si>
+  <si>
+    <t>TCR0011</t>
+  </si>
+  <si>
+    <t>FIX file names and add the new figures here!</t>
+  </si>
+  <si>
+    <t>Also test the simulated data!</t>
   </si>
 </sst>
 </file>
@@ -288,7 +306,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,6 +316,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -314,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -337,6 +361,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,25 +857,25 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>34</v>
@@ -855,146 +883,172 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B31" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="32" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B32" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B33" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B35" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+    <row r="36" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B36" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+    <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B37" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+    <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B40" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B41" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B42" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B43" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B44" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B45" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+    <row r="46" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B46" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+    <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B47" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B48" s="5" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat/doc: Added tests for the new functions, renamed files, and cleaned up the code.
</commit_message>
<xml_diff>
--- a/RCode/VerificationMatrix.xlsx
+++ b/RCode/VerificationMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\R\ButterflyPublicationRepo\GRNP_2020\RCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE95B54-88F3-40B3-A476-F854E0E18B96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959E458D-B361-4C3F-B9BA-557FC3242CDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1485" windowWidth="25170" windowHeight="14715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="96">
   <si>
     <t>File/Function</t>
   </si>
@@ -195,15 +195,9 @@
     <t>The peformance gain vs accuracy loss is tested with TCR0004 - more of a validation. The results look reasonable the slow and fast version are very similar. The function is not technically tested, but the results look good, so we have no reason to doubt that it works.</t>
   </si>
   <si>
-    <t>GenFig1.R</t>
-  </si>
-  <si>
     <t>Difficult to test. We see some things that convince us that it works: The .25 points ends up as expected, although calculated separately. The prediction works as expected, producing reasonably constant values for the predictions. The rest of the code is rather trivial.</t>
   </si>
   <si>
-    <t>GenFig1Data.R</t>
-  </si>
-  <si>
     <t>See GenFig1.R</t>
   </si>
   <si>
@@ -213,24 +207,9 @@
     <t>These are fairly simple plots with results that look as expected. No further verification is deemed necessary.</t>
   </si>
   <si>
-    <t>GenFig3_S7.R</t>
-  </si>
-  <si>
-    <t>GenFig3_S7Data.R</t>
-  </si>
-  <si>
     <t>These plots show complicated things, but all that is calculated in underlying functions with a separate test entry in this verification matrix. The figure code in itself is fairly straight-forward. No explicit testing is deemed necessary.</t>
   </si>
   <si>
-    <t>See GenFig3_S7.R</t>
-  </si>
-  <si>
-    <t>GenFig4.R</t>
-  </si>
-  <si>
-    <t>GenFig4Data.R</t>
-  </si>
-  <si>
     <t>See GenFig4.R</t>
   </si>
   <si>
@@ -246,12 +225,6 @@
     <t>GenFigS1-S3.R</t>
   </si>
   <si>
-    <t>GenFigS6_S8-20Data.R</t>
-  </si>
-  <si>
-    <t>GenFigS6_S8-20.R</t>
-  </si>
-  <si>
     <t>This code is difficult to test and is fairly straight-forward, it calls a lot of prediction methods and saves the data. The produced end results look reasonable. The code has been reviewed. No further testing is deemed necessary.</t>
   </si>
   <si>
@@ -279,10 +252,67 @@
     <t>TCR0011</t>
   </si>
   <si>
-    <t>FIX file names and add the new figures here!</t>
-  </si>
-  <si>
-    <t>Also test the simulated data!</t>
+    <t>GenFig1_3Data.R</t>
+  </si>
+  <si>
+    <t>GenFig1_3.R</t>
+  </si>
+  <si>
+    <t>GenFig4A-C_S23.R</t>
+  </si>
+  <si>
+    <t>See GenFig4A-C_S23.R</t>
+  </si>
+  <si>
+    <t>GenFig4A-C_S23Data.R</t>
+  </si>
+  <si>
+    <t>GenFig4DE.R</t>
+  </si>
+  <si>
+    <t>GenFig4DEData.R</t>
+  </si>
+  <si>
+    <t>GenFig5AB.R</t>
+  </si>
+  <si>
+    <t>GenFig5C-H_S24-S25.R</t>
+  </si>
+  <si>
+    <t>GetFigS6.R</t>
+  </si>
+  <si>
+    <t>GenFigS6Data.R</t>
+  </si>
+  <si>
+    <t>GenFigS7-S21.R</t>
+  </si>
+  <si>
+    <t>GenFigS7-S21Data.R</t>
+  </si>
+  <si>
+    <t>GenFigS22.R</t>
+  </si>
+  <si>
+    <t>GenFigS22Data.R</t>
+  </si>
+  <si>
+    <t>The batch correction in itself can easily be verified graphically in the figure, it is unlikely that the improvements would come if the batch correction didn't work. However, the nearest neighbor calculations should be tested. We check a few things: 1. That the dataset source and coordinates match, i.e. have the same cell ids at the same indices (commented as test 1 in the code, only tested for uncorrected, the code for corrected is identical). The knn calculations are tested with a test case in the code (Test 2).</t>
+  </si>
+  <si>
+    <t>FIg S24 shows that the Seurat processing has worked somewhat at least. In addition, we check that we identified the clusters correctly, see Test 1 and Test 2 in the code. We test that the extracted CU per cluster for cluster 0 matches that explicitly calculated in a different way (Test 3). The rest of the code is difficult to test, but the results look as expected, no large surprises.</t>
+  </si>
+  <si>
+    <t>The code is generally difficult to test, we mostly rely on external R packages. We do test the GC calculation function though (Test 1) and that the mean calculation across groups work for the variables (Test 2)</t>
+  </si>
+  <si>
+    <t>This code is trivial, it just plots the data generated by GenFigS6Data - no tests were deemed needed.</t>
+  </si>
+  <si>
+    <t>We test the function calcFSCM with Test 1 in the code, the function trimZeros with Test 2 in the code, and the large function evaluateCondition with Test 3 in the code. Test 3 also implicitly tests genGeneData. The code for linear interpolation was not formally tested, although it produces reasonable results. The rest of the code is not formally tested, it mainly uses the other functions, the code is not that complicated. The prediction and binomial downsampling functions were not tested, but rather validated as they do improve the classifications in the figures. Estimation of counts per cell was not explicitly tested, although it produced reasonable results. That code is only a few lines.</t>
+  </si>
+  <si>
+    <t>No explicit tests have been done for this code. It is mainly graphical code, although there are some lines about AUC calculations. Those follow the recommended way of using the package, and yield the expected result, so no more tests were deemed necessary.</t>
   </si>
 </sst>
 </file>
@@ -306,7 +336,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,12 +346,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -361,10 +385,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,15 +879,15 @@
         <v>31</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -923,10 +948,10 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -947,108 +972,146 @@
     </row>
     <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B43" s="5" t="s">
+    </row>
+    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A53" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+      <c r="B54" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>